<commit_message>
Only Upazilla Planned Adp
</commit_message>
<xml_diff>
--- a/DAM_Database/For_Risk.xlsx
+++ b/DAM_Database/For_Risk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PortableCompiler\Codes\Dynamic Adaptation Model\DAM\DAM_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20852C2-6F1B-4297-9811-2297401B81E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35435331-C6BB-436A-AA6B-715F8D642301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risk" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="120">
   <si>
     <t>DISTNAME</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Sensitivity</t>
   </si>
   <si>
-    <t>Trainning</t>
-  </si>
-  <si>
-    <t>Growth centre</t>
-  </si>
-  <si>
     <t>Bagerhat</t>
   </si>
   <si>
@@ -194,45 +188,6 @@
     <t>Upazilla</t>
   </si>
   <si>
-    <t>Fishculture (Culture/capture)</t>
-  </si>
-  <si>
-    <t>Livestock (Cattle/Poultry)</t>
-  </si>
-  <si>
-    <t>Non-institutional Loan</t>
-  </si>
-  <si>
-    <t>Safe drinking water Source</t>
-  </si>
-  <si>
-    <t>Irrigation System for crops</t>
-  </si>
-  <si>
-    <t>Homestead Plantation &amp; Vegetation</t>
-  </si>
-  <si>
-    <t>Livelihood Migration</t>
-  </si>
-  <si>
-    <t>Social protection Protection</t>
-  </si>
-  <si>
-    <t>Communication Infrastructure</t>
-  </si>
-  <si>
-    <t>Health care Provider</t>
-  </si>
-  <si>
-    <t>Alternative livelihood Options</t>
-  </si>
-  <si>
-    <t>Microcredit/Organizational support (Emergency Support)</t>
-  </si>
-  <si>
-    <t>Cropping system (Shrim/Crab/Agricultural Crops)</t>
-  </si>
-  <si>
     <t>Planned</t>
   </si>
   <si>
@@ -242,105 +197,18 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Aquatic Resources</t>
-  </si>
-  <si>
-    <t>Mixed Aquaculture</t>
-  </si>
-  <si>
-    <t>Livestock</t>
-  </si>
-  <si>
-    <t>Wet land</t>
-  </si>
-  <si>
     <t>Loan</t>
   </si>
   <si>
-    <t>Fitered water</t>
-  </si>
-  <si>
-    <t>pond sand Filter</t>
-  </si>
-  <si>
-    <t>Rain-water harvesting pond</t>
-  </si>
-  <si>
-    <t>Tap Water</t>
-  </si>
-  <si>
-    <t>Tubewell</t>
-  </si>
-  <si>
-    <t>Shallow Tubewell</t>
-  </si>
-  <si>
-    <t>Deep Tubewell</t>
-  </si>
-  <si>
-    <t>Homestead Plantation</t>
-  </si>
-  <si>
-    <t>Insurance</t>
-  </si>
-  <si>
     <t>Pension</t>
   </si>
   <si>
-    <t>SSNP</t>
-  </si>
-  <si>
-    <t>culvert/bridge</t>
-  </si>
-  <si>
-    <t>Community clinic</t>
-  </si>
-  <si>
-    <t>Floating medicine unit</t>
-  </si>
-  <si>
-    <t>Crab farming</t>
-  </si>
-  <si>
-    <t>dry fish</t>
-  </si>
-  <si>
     <t>Salt farming</t>
   </si>
   <si>
-    <t xml:space="preserve">Agriculture/Relief </t>
-  </si>
-  <si>
-    <t>Fertilizer (Red/Black/white)</t>
-  </si>
-  <si>
-    <t>lime</t>
-  </si>
-  <si>
-    <t>Saline tolerant Plant/fish</t>
-  </si>
-  <si>
-    <t>Seed/ Rice bank</t>
-  </si>
-  <si>
-    <t>Water Hyacinth/ Gobor</t>
-  </si>
-  <si>
-    <t>Cattle</t>
-  </si>
-  <si>
-    <t>Poultry</t>
-  </si>
-  <si>
-    <t>Rain-Water Harvesting</t>
-  </si>
-  <si>
     <t>Saline water treatment plant</t>
   </si>
   <si>
-    <t>Canals</t>
-  </si>
-  <si>
     <t>Livelihood migration</t>
   </si>
   <si>
@@ -350,50 +218,191 @@
     <t>Temporary migration</t>
   </si>
   <si>
-    <t>vocational training</t>
-  </si>
-  <si>
-    <t>indigenous Knowledge</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>Road length</t>
-  </si>
-  <si>
-    <t>Health worker</t>
-  </si>
-  <si>
-    <t>Bazar</t>
-  </si>
-  <si>
-    <t>Hat</t>
-  </si>
-  <si>
     <t>Laboring</t>
   </si>
   <si>
-    <t>shrimp farming/Agriculture</t>
-  </si>
-  <si>
-    <t>Integrated farming/Fishing</t>
-  </si>
-  <si>
-    <t>Cropping Intensity/Gher intensity</t>
-  </si>
-  <si>
-    <t>Access to capture</t>
-  </si>
-  <si>
-    <t>Aquaculture pond</t>
+    <t>Access to capture fish</t>
+  </si>
+  <si>
+    <t>Aquaculture ponds</t>
+  </si>
+  <si>
+    <t>Access to aquatic resources</t>
+  </si>
+  <si>
+    <t>Mixed aquaculture</t>
+  </si>
+  <si>
+    <t>Cattle rearing</t>
+  </si>
+  <si>
+    <t>Livestock place</t>
+  </si>
+  <si>
+    <t>Poultry rearing</t>
+  </si>
+  <si>
+    <t>Available wetland/land for fodder</t>
+  </si>
+  <si>
+    <t>Moneylender (Non-institutional)</t>
+  </si>
+  <si>
+    <t>Filtered water</t>
+  </si>
+  <si>
+    <t>Pond Sand Filter</t>
+  </si>
+  <si>
+    <t>Rainwater harvesting tank</t>
+  </si>
+  <si>
+    <t>Rainwater harvesting pond</t>
+  </si>
+  <si>
+    <t>Tap water</t>
+  </si>
+  <si>
+    <t>Tube well</t>
+  </si>
+  <si>
+    <t>River/Canals</t>
+  </si>
+  <si>
+    <t>Shallow tube well</t>
+  </si>
+  <si>
+    <t>Deep tube well</t>
+  </si>
+  <si>
+    <t>Homestead plantation</t>
+  </si>
+  <si>
+    <t>Vocational/technical training</t>
+  </si>
+  <si>
+    <t>Indigenous knowledge</t>
+  </si>
+  <si>
+    <t>Agriculture/ health/ personal insurance</t>
+  </si>
+  <si>
+    <t>Personal savings</t>
+  </si>
+  <si>
+    <t>Social SafetyNet Program</t>
+  </si>
+  <si>
+    <t>Bridge/Culvert</t>
+  </si>
+  <si>
+    <t>RCC road</t>
+  </si>
+  <si>
+    <t>Number of community clinic</t>
+  </si>
+  <si>
+    <t>Floating medical unit</t>
+  </si>
+  <si>
+    <t>Number of health worker</t>
+  </si>
+  <si>
+    <t>Market/Bazar with hard structure</t>
+  </si>
+  <si>
+    <t>Hat with hard structure</t>
+  </si>
+  <si>
+    <t>Crab fattening</t>
+  </si>
+  <si>
+    <t>Dry fish</t>
+  </si>
+  <si>
+    <t>Shrimp farming</t>
+  </si>
+  <si>
+    <t>Agricultural support (Seed/Fertilizer)</t>
+  </si>
+  <si>
+    <t>Micro-credit from organizations</t>
+  </si>
+  <si>
+    <t>Livestock support (Poultry/ Cattle/ Place)</t>
+  </si>
+  <si>
+    <t>Relief (Rice/Money/Foods)</t>
+  </si>
+  <si>
+    <t>Fertilizer (Red and Black)</t>
+  </si>
+  <si>
+    <t>Integrated farming</t>
+  </si>
+  <si>
+    <t>Lime (CaOH2)</t>
+  </si>
+  <si>
+    <t>Saline tolerant plant/Fish/Crab</t>
+  </si>
+  <si>
+    <t>Seed/Rice bank</t>
+  </si>
+  <si>
+    <t>Water Hyacinth</t>
+  </si>
+  <si>
+    <t>Cropping intensity</t>
+  </si>
+  <si>
+    <t>Fisheries</t>
+  </si>
+  <si>
+    <t>Livestock Farming</t>
+  </si>
+  <si>
+    <t>Safe water drinking sources</t>
+  </si>
+  <si>
+    <t>Irrigation System</t>
+  </si>
+  <si>
+    <t>Plantation</t>
+  </si>
+  <si>
+    <t>Migration</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Social protection system</t>
+  </si>
+  <si>
+    <t>Communication &amp; infrastructure System</t>
+  </si>
+  <si>
+    <t>Health care system</t>
+  </si>
+  <si>
+    <t>Growth center</t>
+  </si>
+  <si>
+    <t>Alternate livelihood options</t>
+  </si>
+  <si>
+    <t>Organizational support</t>
+  </si>
+  <si>
+    <t>Cropping system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +417,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -430,10 +451,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -742,57 +765,57 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" t="s">
-        <v>54</v>
-      </c>
       <c r="J1" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="M1" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="N1" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="O1" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="P1" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="Q1" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="R1" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="S1" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="T1" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="U1" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>400108</v>
@@ -854,10 +877,10 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>400114</v>
@@ -919,10 +942,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>400134</v>
@@ -984,10 +1007,10 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>400138</v>
@@ -1049,10 +1072,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>400156</v>
@@ -1114,10 +1137,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>400158</v>
@@ -1179,10 +1202,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>400160</v>
@@ -1244,10 +1267,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>400173</v>
@@ -1309,10 +1332,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>400177</v>
@@ -1374,10 +1397,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>404104</v>
@@ -1439,10 +1462,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
       </c>
       <c r="C12">
         <v>404109</v>
@@ -1504,10 +1527,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>404111</v>
@@ -1569,10 +1592,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>404123</v>
@@ -1634,10 +1657,10 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>404138</v>
@@ -1699,10 +1722,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>404147</v>
@@ -1764,10 +1787,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>404161</v>
@@ -1829,10 +1852,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>404190</v>
@@ -1894,10 +1917,10 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>404712</v>
@@ -1959,10 +1982,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
       </c>
       <c r="C20">
         <v>404717</v>
@@ -2024,10 +2047,10 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>404730</v>
@@ -2089,10 +2112,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>404740</v>
@@ -2154,10 +2177,10 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>404748</v>
@@ -2219,10 +2242,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>404753</v>
@@ -2284,10 +2307,10 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>404764</v>
@@ -2349,10 +2372,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>404769</v>
@@ -2414,10 +2437,10 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27">
         <v>404775</v>
@@ -2479,10 +2502,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>404794</v>
@@ -2544,10 +2567,10 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>406528</v>
@@ -2609,10 +2632,10 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
         <v>37</v>
-      </c>
-      <c r="B30" t="s">
-        <v>39</v>
       </c>
       <c r="C30">
         <v>406552</v>
@@ -2674,10 +2697,10 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>406576</v>
@@ -2739,10 +2762,10 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>408704</v>
@@ -2804,10 +2827,10 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
         <v>41</v>
-      </c>
-      <c r="B33" t="s">
-        <v>43</v>
       </c>
       <c r="C33">
         <v>408725</v>
@@ -2869,10 +2892,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>408743</v>
@@ -2934,10 +2957,10 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>408747</v>
@@ -2999,10 +3022,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36">
         <v>408782</v>
@@ -3064,10 +3087,10 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37">
         <v>408786</v>
@@ -3129,10 +3152,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>408790</v>
@@ -3201,7 +3224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D04715-CE9B-461D-A343-E58AEA517AF9}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
@@ -3212,15 +3235,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>7.7218795091993683E-2</v>
@@ -3228,7 +3251,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>7.4951670411291915E-2</v>
@@ -3236,7 +3259,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>5.0226077616305709E-2</v>
@@ -3244,7 +3267,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>5.8814821739656215E-2</v>
@@ -3252,7 +3275,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>5.6903982167618314E-2</v>
@@ -3260,7 +3283,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>2.8334162552793786E-2</v>
@@ -3268,7 +3291,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="B8">
         <v>4.6718433551358685E-2</v>
@@ -3276,7 +3299,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="B9">
         <v>4.4974047537971705E-2</v>
@@ -3284,7 +3307,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B10">
         <v>3.6653216402306982E-2</v>
@@ -3292,7 +3315,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="B11">
         <v>2.6596408360212188E-2</v>
@@ -3300,7 +3323,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="B12">
         <v>3.5160725694872469E-2</v>
@@ -3308,7 +3331,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="B13">
         <v>6.0220322994464191E-2</v>
@@ -3316,7 +3339,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B14">
         <v>5.2387918586440214E-2</v>
@@ -3324,7 +3347,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="B15">
         <v>4.8735343811600225E-2</v>
@@ -3332,7 +3355,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="B16">
         <v>0.30210407348111384</v>
@@ -3347,7 +3370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805E8958-582A-4073-BD50-314979B36887}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3358,582 +3383,582 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>115</v>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>0.20094936708860761</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>116</v>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C3" s="1">
         <v>0.33702531645569622</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>68</v>
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
       </c>
       <c r="C4" s="1">
         <v>6.3291139240506328E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>69</v>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C5" s="1">
         <v>0.45569620253164561</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>96</v>
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
       </c>
       <c r="C6" s="1">
         <v>0.36679536679536678</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>70</v>
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="1">
         <v>0.19691119691119693</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>97</v>
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
       </c>
       <c r="C8" s="1">
         <v>0.34362934362934366</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>71</v>
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
       </c>
       <c r="C9" s="1">
         <v>9.2664092664092673E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>72</v>
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>73</v>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>74</v>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>98</v>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C13" s="1">
         <v>0.63419117647058831</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>75</v>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>99</v>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="1">
         <v>0.36580882352941174</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>76</v>
+      <c r="A16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>77</v>
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>100</v>
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C18" s="1">
         <v>0.92814371257485029</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>78</v>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C19" s="1">
         <v>7.1856287425149712E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>79</v>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>101</v>
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
       </c>
       <c r="C22" s="1">
         <v>0.78804347826086951</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
         <v>58</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="C23" s="1">
         <v>0.10869565217391305</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>103</v>
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
       </c>
       <c r="C24" s="1">
         <v>0.10326086956521739</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>104</v>
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
       </c>
       <c r="C25" s="1">
         <v>0.75870646766169159</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>105</v>
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
       </c>
       <c r="C26" s="1">
         <v>0.24129353233830844</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>81</v>
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
       </c>
       <c r="C27" s="1">
         <v>1.8633540372670811E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>82</v>
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
       </c>
       <c r="C28" s="1">
         <v>2.4844720496894412E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>106</v>
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
       </c>
       <c r="C29" s="1">
         <v>0.72670807453416142</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>83</v>
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
       </c>
       <c r="C30" s="1">
         <v>0.22981366459627334</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>84</v>
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
       </c>
       <c r="C31" s="1">
         <v>0.22764227642276424</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>107</v>
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
       </c>
       <c r="C32" s="1">
         <v>0.77235772357723576</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>85</v>
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>86</v>
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>108</v>
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>109</v>
+      <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
       </c>
       <c r="C36" s="1">
         <v>0.34649910233393172</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>110</v>
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
       </c>
       <c r="C37" s="1">
         <v>0.65350089766606823</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>87</v>
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>88</v>
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>111</v>
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
       </c>
       <c r="C40" s="1">
         <v>0.10344827586206895</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>112</v>
+      <c r="A41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
       </c>
       <c r="C41" s="1">
         <v>0.89655172413793105</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>89</v>
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>90</v>
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
       </c>
       <c r="C43" s="1">
         <v>0.12857142857142859</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>82</v>
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
       </c>
       <c r="C44" s="1">
         <v>0.1357142857142857</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>70</v>
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
       </c>
       <c r="C45" s="1">
         <v>8.2142857142857156E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>83</v>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="C46" s="1">
         <v>0.65357142857142858</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>91</v>
+      <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
       </c>
       <c r="C47" s="1">
         <v>0.2076271186440678</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>113</v>
+      <c r="A48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
       </c>
       <c r="C48" s="1">
         <v>0.15466101694915255</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>92</v>
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
       </c>
       <c r="C49" s="1">
         <v>0.2309322033898305</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>93</v>
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
       </c>
       <c r="C50" s="1">
         <v>7.6271186440677985E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>94</v>
+      <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
       </c>
       <c r="C51" s="1">
         <v>7.0621468926553683E-4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>95</v>
+      <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
       </c>
       <c r="C52" s="1">
         <v>0.19209039548022599</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>114</v>
+      <c r="A53" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
       </c>
       <c r="C53" s="1">
         <v>0.13771186440677968</v>

</xml_diff>